<commit_message>
Added Cardiometabolic health markers to the analyses
</commit_message>
<xml_diff>
--- a/Data/Mol_raw_data.xlsx
+++ b/Data/Mol_raw_data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Marria Paulina Correa/Visualisation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C13017F-C652-0846-8863-C0A8B13B99EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2575D-CC66-2643-B6E6-CF487797E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" activeTab="3" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
   </bookViews>
   <sheets>
     <sheet name="Females" sheetId="1" r:id="rId1"/>
     <sheet name="Males" sheetId="2" r:id="rId2"/>
+    <sheet name="Female_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Males_2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>FEMALES (n=100)</t>
   </si>
@@ -118,6 +120,75 @@
   </si>
   <si>
     <t>TNFa</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Waist circ</t>
+  </si>
+  <si>
+    <t>WtHt</t>
+  </si>
+  <si>
+    <t>Fat mass</t>
+  </si>
+  <si>
+    <t>FMC1</t>
+  </si>
+  <si>
+    <t>FMC2*</t>
+  </si>
+  <si>
+    <t>FMC3*</t>
+  </si>
+  <si>
+    <t>Systolic BP</t>
+  </si>
+  <si>
+    <t>Diastolic BP</t>
+  </si>
+  <si>
+    <t>PWV</t>
+  </si>
+  <si>
+    <t>CIMTL</t>
+  </si>
+  <si>
+    <t>CIMTR</t>
+  </si>
+  <si>
+    <t>Glycemia</t>
+  </si>
+  <si>
+    <t>HOMA-IR</t>
+  </si>
+  <si>
+    <t>Triglycerides</t>
+  </si>
+  <si>
+    <t>HDL-Chol*</t>
+  </si>
+  <si>
+    <t>HOMA-β</t>
+  </si>
+  <si>
+    <t>MetS score</t>
+  </si>
+  <si>
+    <t>Liver score</t>
+  </si>
+  <si>
+    <t>Fat Mass</t>
+  </si>
+  <si>
+    <t>SBP</t>
+  </si>
+  <si>
+    <t>DBP</t>
   </si>
 </sst>
 </file>
@@ -129,7 +200,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +216,17 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
@@ -169,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -179,11 +261,265 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
@@ -322,28 +658,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D0686F-E73D-9A4C-AC83-D71ECC8606B4}" name="Tabla1" displayName="Tabla1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D0686F-E73D-9A4C-AC83-D71ECC8606B4}" name="Tabla1" displayName="Tabla1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:D22" xr:uid="{62D0686F-E73D-9A4C-AC83-D71ECC8606B4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DF7DB22F-F45A-D54F-8AB2-61B6A9D35B88}" name="FEMALES (n=100)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8055896A-07FE-EC43-9CB3-B3615966E1EE}" name="TG1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{CFCE73E3-D823-AA46-89D3-3C28AB6D9BBB}" name="TG2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A497DB54-A8FB-3E4C-A452-1E967BDE46EB}" name="TG3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{DF7DB22F-F45A-D54F-8AB2-61B6A9D35B88}" name="FEMALES (n=100)" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{8055896A-07FE-EC43-9CB3-B3615966E1EE}" name="TG1" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{CFCE73E3-D823-AA46-89D3-3C28AB6D9BBB}" name="TG2" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{A497DB54-A8FB-3E4C-A452-1E967BDE46EB}" name="TG3" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CD495AD2-75BD-6C45-A1FC-1B4739D5E68B}" name="Tabla13" displayName="Tabla13" ref="A1:D22" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CD495AD2-75BD-6C45-A1FC-1B4739D5E68B}" name="Tabla13" displayName="Tabla13" ref="A1:D22" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:D22" xr:uid="{CD495AD2-75BD-6C45-A1FC-1B4739D5E68B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{80B8B741-D8D6-BA44-BD0D-4271987FB43D}" name="MALES (n=105)"/>
-    <tableColumn id="2" xr3:uid="{019F1107-09DC-FE40-B079-6EE2CB45FCF9}" name="TG1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4875EC7F-595E-6848-A2C2-6553C845DA07}" name="TG2" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D9C41602-E08F-5F4D-8A2E-1669A12B1F3F}" name="TG3" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{019F1107-09DC-FE40-B079-6EE2CB45FCF9}" name="TG1" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{4875EC7F-595E-6848-A2C2-6553C845DA07}" name="TG2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{D9C41602-E08F-5F4D-8A2E-1669A12B1F3F}" name="TG3" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{673E7DD9-EC6A-2342-9325-CD42F6B7D0BD}" name="Tabla14" displayName="Tabla14" ref="A1:D41" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A1:D41" xr:uid="{673E7DD9-EC6A-2342-9325-CD42F6B7D0BD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EC0788BB-541F-684A-8CE2-BEEEC109F77F}" name="Columna1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D54030EC-BFD2-324A-8C34-675B5FB90969}" name="TG1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{7D95234B-300E-864E-A006-8983562B5A9F}" name="TG2" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A44C40D0-62B4-8B4E-ACAB-740BCF8374CB}" name="TG3" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4518305E-A2D5-C64D-B6ED-7F732C08B6B5}" name="Tabla15" displayName="Tabla15" ref="A1:D41" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D41" xr:uid="{4518305E-A2D5-C64D-B6ED-7F732C08B6B5}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A5EE1A60-28FA-4449-87A8-441141FD9290}" name="Columna1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{19FC57F3-0D75-944D-AC1C-2C48731B04AC}" name="TG1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C2E12C30-9812-194E-BE03-6EF9A3275AFE}" name="TG2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1FF2E165-0321-0544-9A44-F26C1EEF5171}" name="TG3" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -666,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C3728-47BA-3949-A281-2B29FCD926BD}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1318,4 +1680,1193 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8457E20-D81E-794A-A2F5-9B987CF62003}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10">
+        <v>22.7</v>
+      </c>
+      <c r="C2" s="10">
+        <v>34.5</v>
+      </c>
+      <c r="D2" s="10">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="10">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="C3" s="10">
+        <v>98.2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>108.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.46</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="10">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="C5" s="10">
+        <v>47</v>
+      </c>
+      <c r="D5" s="10">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.47</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="D7" s="10">
+        <v>3.2258064516129035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.2820512820512819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10">
+        <v>106</v>
+      </c>
+      <c r="C9" s="10">
+        <v>121</v>
+      </c>
+      <c r="D9" s="10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="10">
+        <v>76</v>
+      </c>
+      <c r="C10" s="10">
+        <v>77</v>
+      </c>
+      <c r="D10" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C11" s="10">
+        <v>5.3</v>
+      </c>
+      <c r="D11" s="10">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.46</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.47</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="10">
+        <v>87.5</v>
+      </c>
+      <c r="C14" s="10">
+        <v>90</v>
+      </c>
+      <c r="D14" s="10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="C15" s="10">
+        <v>3.2</v>
+      </c>
+      <c r="D15" s="10">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="10">
+        <v>63.9</v>
+      </c>
+      <c r="C16" s="10">
+        <v>98.4</v>
+      </c>
+      <c r="D16" s="10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="11">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="C17" s="11">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="D17" s="11">
+        <v>4.1399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="10">
+        <v>152.4</v>
+      </c>
+      <c r="C18" s="10">
+        <v>248.7</v>
+      </c>
+      <c r="D18" s="10">
+        <v>246.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="10">
+        <v>27.5</v>
+      </c>
+      <c r="C21" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D21" s="10">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="10">
+        <v>0.12330456226880396</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.13440860215053763</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1.02</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4.58</v>
+      </c>
+      <c r="D23" s="10">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1.59</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1.62</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1.73</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2.62</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.61728395061728392</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="10">
+        <v>11</v>
+      </c>
+      <c r="C27" s="10">
+        <v>11.3</v>
+      </c>
+      <c r="D27" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="10">
+        <v>7.6</v>
+      </c>
+      <c r="C28" s="10">
+        <v>9.33</v>
+      </c>
+      <c r="D28" s="10">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C29" s="10">
+        <v>14.9</v>
+      </c>
+      <c r="D29" s="10">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="12">
+        <v>7.575757575757576E-3</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1.1235955056179775E-2</v>
+      </c>
+      <c r="D30" s="12">
+        <v>1.2987012987012988E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="12">
+        <v>9.5602294455066918E-4</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1.1904761904761906E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="10">
+        <v>275</v>
+      </c>
+      <c r="C32" s="10">
+        <v>284</v>
+      </c>
+      <c r="D32" s="10">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="10">
+        <v>1084</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1214</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="10">
+        <v>5.2</v>
+      </c>
+      <c r="C34" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="D34" s="10">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="10">
+        <v>2293</v>
+      </c>
+      <c r="C35" s="10">
+        <v>2348</v>
+      </c>
+      <c r="D35" s="10">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10">
+        <v>184.2</v>
+      </c>
+      <c r="C36" s="10">
+        <v>189</v>
+      </c>
+      <c r="D36" s="10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="10">
+        <v>2.1834061135371178E-3</v>
+      </c>
+      <c r="C37" s="10">
+        <v>2.2779043280182231E-3</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2.403846153846154E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="10">
+        <v>11.6</v>
+      </c>
+      <c r="C38" s="10">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D38" s="10">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="10">
+        <v>167.2</v>
+      </c>
+      <c r="C39" s="10">
+        <v>196.7</v>
+      </c>
+      <c r="D39" s="10">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="10">
+        <v>4.29</v>
+      </c>
+      <c r="C40" s="10">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D40" s="10">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="10">
+        <v>4504</v>
+      </c>
+      <c r="C41" s="10">
+        <v>14210</v>
+      </c>
+      <c r="D41" s="10">
+        <v>16544</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A887BF0-E66F-6840-948B-34D6B9F8897A}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="9">
+        <v>23.9</v>
+      </c>
+      <c r="C2" s="9">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9">
+        <v>83.7</v>
+      </c>
+      <c r="C3" s="9">
+        <v>106.2</v>
+      </c>
+      <c r="D3" s="9">
+        <v>112.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9">
+        <v>27.3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>39.6</v>
+      </c>
+      <c r="D5" s="9">
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9">
+        <v>3.12</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3.57</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1.28</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1.56</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="9">
+        <v>121</v>
+      </c>
+      <c r="C9" s="9">
+        <v>128</v>
+      </c>
+      <c r="D9" s="9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="9">
+        <v>74</v>
+      </c>
+      <c r="C10" s="9">
+        <v>77</v>
+      </c>
+      <c r="D10" s="9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9">
+        <v>5.2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.46</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="10">
+        <v>91</v>
+      </c>
+      <c r="C14" s="10">
+        <v>95</v>
+      </c>
+      <c r="D14" s="10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C15" s="10">
+        <v>3.7</v>
+      </c>
+      <c r="D15" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="10">
+        <v>152.9</v>
+      </c>
+      <c r="C16" s="10">
+        <v>225.2</v>
+      </c>
+      <c r="D16" s="10">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="10">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="C17" s="10">
+        <v>99.2</v>
+      </c>
+      <c r="D17" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10">
+        <v>4</v>
+      </c>
+      <c r="D20" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="10">
+        <v>28.4</v>
+      </c>
+      <c r="C21" s="10">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D21" s="10">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="10">
+        <v>0.12658227848101264</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.13477088948787061</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.13513513513513511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1.74</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1.67</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1.77</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.54347826086956519</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="10">
+        <v>9.07</v>
+      </c>
+      <c r="C27" s="10">
+        <v>9.15</v>
+      </c>
+      <c r="D27" s="10">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="10">
+        <v>9.6</v>
+      </c>
+      <c r="C28" s="10">
+        <v>14.4</v>
+      </c>
+      <c r="D28" s="10">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="10">
+        <v>8.130081300813009E-3</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1.0309278350515464E-2</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1.1235955056179775E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1.0493179433368311E-3</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.2594458438287153E-3</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1.3054830287206266E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="10">
+        <v>258</v>
+      </c>
+      <c r="C31" s="10">
+        <v>270</v>
+      </c>
+      <c r="D31" s="10">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="10">
+        <v>1105</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1210</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="10">
+        <v>4.8</v>
+      </c>
+      <c r="C33" s="10">
+        <v>5.4</v>
+      </c>
+      <c r="D33" s="10">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="10">
+        <v>2087</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2266</v>
+      </c>
+      <c r="D34" s="10">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="10">
+        <v>190</v>
+      </c>
+      <c r="C35" s="10">
+        <v>201.1</v>
+      </c>
+      <c r="D35" s="10">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="10">
+        <v>2.0964360587002098E-3</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2.1276595744680851E-3</v>
+      </c>
+      <c r="D36" s="10">
+        <v>2.3364485981308409E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="10">
+        <v>11.6</v>
+      </c>
+      <c r="C37" s="10">
+        <v>16.7</v>
+      </c>
+      <c r="D37" s="10">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="10">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="C38" s="10">
+        <v>193.8</v>
+      </c>
+      <c r="D38" s="10">
+        <v>209.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1594</v>
+      </c>
+      <c r="C39" s="10">
+        <v>3586</v>
+      </c>
+      <c r="D39" s="10">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="C40" s="10">
+        <v>11.8</v>
+      </c>
+      <c r="D40" s="10">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="10">
+        <v>3.95</v>
+      </c>
+      <c r="C41" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="D41" s="10">
+        <v>4.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added nbclust, clusters, and colors for markers
</commit_message>
<xml_diff>
--- a/Data/Mol_raw_data.xlsx
+++ b/Data/Mol_raw_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Marria Paulina Correa/Visualisation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2575D-CC66-2643-B6E6-CF487797E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318D9F6-6DA3-A844-A3BA-02E5161DF863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" activeTab="3" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
   </bookViews>
   <sheets>
     <sheet name="Females" sheetId="1" r:id="rId1"/>
     <sheet name="Males" sheetId="2" r:id="rId2"/>
     <sheet name="Female_2" sheetId="3" r:id="rId3"/>
     <sheet name="Males_2" sheetId="4" r:id="rId4"/>
+    <sheet name="Markers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="55">
   <si>
     <t>FEMALES (n=100)</t>
   </si>
@@ -189,6 +190,21 @@
   </si>
   <si>
     <t>DBP</t>
+  </si>
+  <si>
+    <t>Molecular analytes</t>
+  </si>
+  <si>
+    <t>Cardiometabolic health markers</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Males</t>
+  </si>
+  <si>
+    <t>Females</t>
   </si>
 </sst>
 </file>
@@ -200,7 +216,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,16 +246,40 @@
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -247,11 +287,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -266,6 +328,17 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2283,7 +2356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A887BF0-E66F-6840-948B-34D6B9F8897A}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2869,4 +2942,496 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5E538A-7D24-404D-9270-8DB55D496FF9}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="23"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalising analyses and figures
</commit_message>
<xml_diff>
--- a/Data/Mol_raw_data.xlsx
+++ b/Data/Mol_raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Marria Paulina Correa/Visualisation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318D9F6-6DA3-A844-A3BA-02E5161DF863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DF277A-D898-2B49-ACF9-2A4FC21AF8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" activeTab="4" xr2:uid="{21689FDD-5DBC-A34E-AF92-5C6F13429811}"/>
   </bookViews>
   <sheets>
     <sheet name="Females" sheetId="1" r:id="rId1"/>
@@ -2949,7 +2949,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>